<commit_message>
Modified to support multibrowser testing
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12648" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSteps" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="2"/>
+    <sheet name="Settings" r:id="rId3" sheetId="3"/>
   </sheets>
+  <definedNames>
+    <definedName name="ActionKeywords">Settings!$D$2:$D$24</definedName>
+    <definedName name="HomePageObjects">Settings!$B$2:$B$19</definedName>
+    <definedName name="LoginPageObjects">Settings!$C$2:$C$16</definedName>
+    <definedName name="PageName">Settings!$A$2:$A$21</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -183,12 +190,43 @@
   <si>
     <t>FAIL</t>
   </si>
+  <si>
+    <t>prayatna.khata</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>Data_Set</t>
+  </si>
+  <si>
+    <t>PageName</t>
+  </si>
+  <si>
+    <t>LoginPage</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>HomePageObjects</t>
+  </si>
+  <si>
+    <t>LoginPageObjects</t>
+  </si>
+  <si>
+    <t>ActionKeywords</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +255,14 @@
       <color rgb="FF303030"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,24 +297,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -285,10 +337,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -323,7 +375,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -358,7 +410,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -452,21 +504,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -483,7 +535,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -535,31 +587,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="38.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -576,10 +629,13 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -594,10 +650,13 @@
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -611,11 +670,12 @@
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -631,11 +691,12 @@
       <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -652,10 +713,13 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -671,11 +735,14 @@
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -691,11 +758,12 @@
       <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -709,11 +777,12 @@
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -729,11 +798,12 @@
       <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -749,11 +819,12 @@
       <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -767,30 +838,34 @@
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="F6" xr:uid="{42FC1814-BEDE-43F6-90F1-2D7649C3D48A}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{217D7FA9-362F-4501-ACA4-EA35E6C10DBF}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{217D7FA9-362F-4501-ACA4-EA35E6C10DBF}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="11.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="16.21875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="9.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="6.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,7 +908,114 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5883BD1B-0151-421C-A1A2-56E64FD093C5}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.77734375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>